<commit_message>
CharactersCreator and CharactersCreatorForm Ready
</commit_message>
<xml_diff>
--- a/D-DHelper/D-DHelper/Materials/CharactersBase.xlsx
+++ b/D-DHelper/D-DHelper/Materials/CharactersBase.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -570,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH1" activeCellId="1" sqref="AI1 AH1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,6 +692,62 @@
       </c>
     </row>
     <row r="2" spans="1:35" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="9:33" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>35</v>
+      </c>
+      <c r="P22" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>35</v>
+      </c>
+      <c r="R22" t="s">
+        <v>35</v>
+      </c>
+      <c r="S22" t="s">
+        <v>35</v>
+      </c>
+      <c r="U22" t="s">
+        <v>35</v>
+      </c>
+      <c r="V22" t="s">
+        <v>35</v>
+      </c>
+      <c r="W22" t="s">
+        <v>35</v>
+      </c>
+      <c r="X22" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>